<commit_message>
Changed graphs, so the accuracy on the scale maximum is 100% and not more than that
</commit_message>
<xml_diff>
--- a/evaluation data/Accuracy evaluation.xlsx
+++ b/evaluation data/Accuracy evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\new pytorchfi\pytorchfi\evaluation data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DD57FE-AE43-42AA-B535-DDA7389A14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F6B51F-0F6D-4C2C-AAE2-3A8726AF2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
+    <workbookView xWindow="12645" yWindow="555" windowWidth="15555" windowHeight="14715" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiply all values with 1+e" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="47">
   <si>
     <t>Epsilon</t>
   </si>
@@ -79,15 +79,6 @@
     <t>densenet121 with CIFAR100 &amp; epsilon mul</t>
   </si>
   <si>
-    <t>densenet121 with MNIST &amp; bit flip</t>
-  </si>
-  <si>
-    <t>densenet121 with CIFAR10 &amp; bit flip</t>
-  </si>
-  <si>
-    <t>densenet121 with CIFAR100 &amp; bit flip</t>
-  </si>
-  <si>
     <t>Mobilenetv2 Tests</t>
   </si>
   <si>
@@ -106,15 +97,6 @@
     <t>googlenet with CIFAR100 &amp; epsilon mul</t>
   </si>
   <si>
-    <t>googlenet with MNIST &amp; bit flip</t>
-  </si>
-  <si>
-    <t>googlenet with CIFAR10 &amp; bit flip</t>
-  </si>
-  <si>
-    <t>googlenet with CIFAR100 &amp; bit flip</t>
-  </si>
-  <si>
     <t>Inception_v3 Tests</t>
   </si>
   <si>
@@ -125,15 +107,6 @@
   </si>
   <si>
     <t>inception_v3 with CIFAR100 &amp; epsilon mul</t>
-  </si>
-  <si>
-    <t>inception_v3 with MNIST &amp; bit flip</t>
-  </si>
-  <si>
-    <t>inception_v3 with CIFAR10 &amp; bit flip</t>
-  </si>
-  <si>
-    <t>inception_v3 with CIFAR100 &amp; bit flip</t>
   </si>
   <si>
     <t>Resnet18 Tests</t>
@@ -148,15 +121,6 @@
     <t>resnet18 with CIFAR100 &amp; epsilon mul</t>
   </si>
   <si>
-    <t>resnet18 with MNIST &amp; bit flip</t>
-  </si>
-  <si>
-    <t>resnet18 with CIFAR10 &amp; bit flip</t>
-  </si>
-  <si>
-    <t>resnet18 with CIFAR100 &amp; bit flip</t>
-  </si>
-  <si>
     <t>Squeezenet1_0 Tests</t>
   </si>
   <si>
@@ -169,15 +133,6 @@
     <t>squeezenet1_0 with CIFAR100 &amp; epsilon mul</t>
   </si>
   <si>
-    <t>squeezenet1_0 with MNIST &amp; bit flip</t>
-  </si>
-  <si>
-    <t>squeezenet1_0 with CIFAR10 &amp; bit flip</t>
-  </si>
-  <si>
-    <t>squeezenet1_0 with CIFAR100 &amp; bit flip</t>
-  </si>
-  <si>
     <t>Squeezenet1_1 Tests</t>
   </si>
   <si>
@@ -188,15 +143,6 @@
   </si>
   <si>
     <t>squeezenet1_1 with CIFAR100 &amp; epsilon mul</t>
-  </si>
-  <si>
-    <t>squeezenet1_1 with MNIST &amp; bit flip</t>
-  </si>
-  <si>
-    <t>squeezenet1_1 with CIFAR10 &amp; bit flip</t>
-  </si>
-  <si>
-    <t>squeezenet1_1 with CIFAR100 &amp; bit flip</t>
   </si>
   <si>
     <t>original models with MNIST</t>
@@ -654,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B82504A-91A0-4B5A-BF2F-634626D37FD7}">
   <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="R65" sqref="R65"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +618,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -695,7 +641,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1227,7 +1173,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1763,7 +1709,7 @@
     </row>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1778,19 +1724,19 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
       <c r="E42" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="4"/>
       <c r="I42" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="5"/>
@@ -2291,7 +2237,7 @@
     </row>
     <row r="60" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -2306,19 +2252,19 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="4"/>
       <c r="E61" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="4"/>
       <c r="I61" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
@@ -2819,7 +2765,7 @@
     </row>
     <row r="79" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -2834,19 +2780,19 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="4"/>
       <c r="E80" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F80" s="5"/>
       <c r="G80" s="5"/>
       <c r="H80" s="4"/>
       <c r="I80" s="5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J80" s="5"/>
       <c r="K80" s="5"/>
@@ -3349,7 +3295,7 @@
     </row>
     <row r="98" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3364,19 +3310,19 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="4"/>
       <c r="E99" s="5" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F99" s="5"/>
       <c r="G99" s="5"/>
       <c r="H99" s="4"/>
       <c r="I99" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
@@ -3879,7 +3825,7 @@
     </row>
     <row r="117" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -3894,19 +3840,19 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="4"/>
       <c r="E118" s="5" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="F118" s="5"/>
       <c r="G118" s="5"/>
       <c r="H118" s="4"/>
       <c r="I118" s="5" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="J118" s="5"/>
       <c r="K118" s="5"/>
@@ -4409,38 +4355,38 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="E137" s="5" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
       <c r="I137" s="5" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="J137" s="5"/>
       <c r="K137" s="5"/>
     </row>
     <row r="138" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B138"/>
       <c r="C138" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F138"/>
       <c r="G138" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="J138"/>
       <c r="K138" s="3" t="s">
@@ -4449,21 +4395,21 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C139" s="2">
         <f>A6</f>
         <v>96.597999999999999</v>
       </c>
       <c r="E139" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="G139" s="2">
         <f>E6</f>
         <v>75.59</v>
       </c>
       <c r="I139" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="K139" s="2">
         <f>I6</f>
@@ -4472,21 +4418,21 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C140" s="2">
         <f>A25</f>
         <v>93.378</v>
       </c>
       <c r="E140" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="G140" s="2">
         <f>E25</f>
         <v>74.527999999999992</v>
       </c>
       <c r="I140" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="K140" s="2">
         <f>I25</f>
@@ -4495,21 +4441,21 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C141" s="2">
         <f>A44</f>
         <v>97.001999999999995</v>
       </c>
       <c r="E141" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="G141" s="2">
         <f>E44</f>
         <v>81.337999999999994</v>
       </c>
       <c r="I141" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="K141" s="2">
         <f>I44</f>
@@ -4518,21 +4464,21 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C142" s="2">
         <f>A63</f>
         <v>97.97</v>
       </c>
       <c r="E142" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G142" s="2">
         <f>E63</f>
         <v>90.92</v>
       </c>
       <c r="I142" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="K142" s="2">
         <f>I63</f>
@@ -4541,21 +4487,21 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C143" s="2">
         <f>A82</f>
         <v>95.24</v>
       </c>
       <c r="E143" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G143" s="2">
         <f>E82</f>
         <v>85.265999999999991</v>
       </c>
       <c r="I143" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="K143" s="2">
         <f>I82</f>
@@ -4564,21 +4510,21 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C144" s="2">
         <f>A101</f>
         <v>16.669999999999998</v>
       </c>
       <c r="E144" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G144" s="2">
         <f>E101</f>
         <v>39.391999999999996</v>
       </c>
       <c r="I144" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="K144" s="2">
         <f>I101</f>
@@ -4587,21 +4533,21 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C145" s="2">
         <f>A120</f>
         <v>11.032</v>
       </c>
       <c r="E145" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="G145" s="2">
         <f>E120</f>
         <v>17.494</v>
       </c>
       <c r="I145" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="K145" s="2">
         <f>I120</f>
@@ -4662,17 +4608,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A2FD27-2957-4E5E-9083-A23CA00D16E3}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:K34"/>
+      <selection activeCell="I4" sqref="I4:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -4741,7 +4692,7 @@
         <v>61.793999999999997</v>
       </c>
       <c r="B4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>57.05+66.61+66.31+61.29+57.71</f>
@@ -4752,592 +4703,373 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="2">
         <f>K4/5</f>
         <v>0</v>
       </c>
       <c r="J4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f t="shared" ref="A5:A19" si="0">C5/5</f>
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E19" si="1">G5/5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2">
+        <f t="shared" ref="I5:I19" si="2">K5/5</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" t="s">
-        <v>2</v>
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f>C9/5</f>
-        <v>69.908000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <f>72.65+68.02+67.25+71.25+70.37</f>
-        <v>349.54</v>
+        <v>5</v>
       </c>
       <c r="E9" s="2">
-        <f>G9/5</f>
-        <v>36.381999999999998</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f>26.2+41.78+31.93+38.66+43.34</f>
-        <v>181.91</v>
+        <v>5</v>
       </c>
       <c r="I9" s="2">
-        <f>K9/5</f>
-        <v>8.2359999999999989</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <f>5.92+9.9+6.9+9.01+9.45</f>
-        <v>41.179999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>8</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <v>9</v>
       </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="I13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
         <v>9</v>
-      </c>
-      <c r="K13" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f>C14/5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="B14" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
-        <f>G14/5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I14" s="2">
-        <f>K14/5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>11</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>12</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>13</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B18" s="2">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f>C19/5</f>
-        <v>75.784000000000006</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <f>76.4+74.2+76+76.13+76.19</f>
-        <v>378.92</v>
+        <v>15</v>
       </c>
       <c r="E19" s="2">
-        <f>G19/5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I19" s="2">
-        <f>K19/5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <f>C24/5</f>
-        <v>71.496000000000009</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <f>73.41+74.45+62.36+73.88+73.38</f>
-        <v>357.48</v>
-      </c>
-      <c r="E24" s="2">
-        <f>G24/5</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>1</v>
-      </c>
-      <c r="I24" s="2">
-        <f>K24/5</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="E27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <f>C29/5</f>
-        <v>13.931999999999999</v>
-      </c>
-      <c r="B29" s="2">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <f>11.21+14.65+19.25+10.39+14.16</f>
-        <v>69.66</v>
-      </c>
-      <c r="E29" s="2">
-        <f>G29/5</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <f>K29/5</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <f>C34/5</f>
-        <v>0</v>
-      </c>
-      <c r="B34" s="2">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2">
-        <f>G34/5</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="I34" s="2">
-        <f>K34/5</f>
-        <v>0</v>
-      </c>
-      <c r="J34" s="2">
-        <v>1</v>
-      </c>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A7:C7"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="I22:K22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated bitflip function again, so it works correctly
</commit_message>
<xml_diff>
--- a/evaluation data/Accuracy evaluation.xlsx
+++ b/evaluation data/Accuracy evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\new pytorchfi\pytorchfi\evaluation data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\github pytorchfi\pytorchfi\evaluation data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F6B51F-0F6D-4C2C-AAE2-3A8726AF2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13399B4E-FC3B-4A0F-9B6E-E6092A64A52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12645" yWindow="555" windowWidth="15555" windowHeight="14715" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
+    <workbookView xWindow="12645" yWindow="555" windowWidth="15555" windowHeight="14715" firstSheet="1" activeTab="2" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiply all values with 1+e" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="51">
   <si>
     <t>Epsilon</t>
   </si>
@@ -180,6 +180,18 @@
   <si>
     <t>Praktischer Part - Robustness und Fault tolerance</t>
   </si>
+  <si>
+    <t>Googlenet with MNIST &amp; bit flip</t>
+  </si>
+  <si>
+    <t>Googlenet with CIFAR10 &amp; bit flip</t>
+  </si>
+  <si>
+    <t>Googlenet with CIFAR100 &amp; bit flip</t>
+  </si>
+  <si>
+    <t>Bit flipped</t>
+  </si>
 </sst>
 </file>
 
@@ -255,13 +267,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -600,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B82504A-91A0-4B5A-BF2F-634626D37FD7}">
   <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:B77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,19 +629,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -655,23 +667,23 @@
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1187,23 +1199,23 @@
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1723,23 +1735,23 @@
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="5" t="s">
+      <c r="E42" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
     </row>
     <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -2251,23 +2263,23 @@
       <c r="K60" s="6"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
       <c r="D61" s="4"/>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
       <c r="H61" s="4"/>
-      <c r="I61" s="5" t="s">
+      <c r="I61" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
     </row>
     <row r="62" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -2779,23 +2791,23 @@
       <c r="K79" s="6"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
       <c r="D80" s="4"/>
-      <c r="E80" s="5" t="s">
+      <c r="E80" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
       <c r="H80" s="4"/>
-      <c r="I80" s="5" t="s">
+      <c r="I80" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
@@ -3309,23 +3321,23 @@
       <c r="K98" s="6"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B99" s="5"/>
-      <c r="C99" s="5"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="5" t="s">
+      <c r="E99" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
       <c r="H99" s="4"/>
-      <c r="I99" s="5" t="s">
+      <c r="I99" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
@@ -3839,23 +3851,23 @@
       <c r="K117" s="6"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+      <c r="A118" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
       <c r="D118" s="4"/>
-      <c r="E118" s="5" t="s">
+      <c r="E118" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
       <c r="H118" s="4"/>
-      <c r="I118" s="5" t="s">
+      <c r="I118" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J118" s="5"/>
-      <c r="K118" s="5"/>
+      <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
@@ -4354,21 +4366,21 @@
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
+      <c r="A137" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B137" s="5"/>
-      <c r="C137" s="5"/>
-      <c r="E137" s="5" t="s">
+      <c r="B137" s="7"/>
+      <c r="C137" s="7"/>
+      <c r="E137" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F137" s="5"/>
-      <c r="G137" s="5"/>
-      <c r="I137" s="5" t="s">
+      <c r="F137" s="7"/>
+      <c r="G137" s="7"/>
+      <c r="I137" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J137" s="5"/>
-      <c r="K137" s="5"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
     </row>
     <row r="138" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
@@ -4556,6 +4568,29 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A137:C137"/>
+    <mergeCell ref="E137:G137"/>
+    <mergeCell ref="I137:K137"/>
+    <mergeCell ref="A117:K117"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="E118:G118"/>
+    <mergeCell ref="I118:K118"/>
+    <mergeCell ref="A98:K98"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="E99:G99"/>
+    <mergeCell ref="I99:K99"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A80:C80"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="I80:K80"/>
+    <mergeCell ref="A60:K60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="I61:K61"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="I42:K42"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A22:K22"/>
@@ -4565,29 +4600,6 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="I4:K4"/>
-    <mergeCell ref="A60:K60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="I61:K61"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="A98:K98"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="E99:G99"/>
-    <mergeCell ref="I99:K99"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="I80:K80"/>
-    <mergeCell ref="A137:C137"/>
-    <mergeCell ref="E137:G137"/>
-    <mergeCell ref="I137:K137"/>
-    <mergeCell ref="A117:K117"/>
-    <mergeCell ref="A118:C118"/>
-    <mergeCell ref="E118:G118"/>
-    <mergeCell ref="I118:K118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -4608,10 +4620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A2FD27-2957-4E5E-9083-A23CA00D16E3}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4637,23 +4649,23 @@
       <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -4689,14 +4701,10 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>C4/5</f>
-        <v>61.793999999999997</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
-      </c>
-      <c r="C4">
-        <f>57.05+66.61+66.31+61.29+57.71</f>
-        <v>308.96999999999997</v>
       </c>
       <c r="E4" s="2">
         <f>G4/5</f>
@@ -4989,7 +4997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5012,7 +5020,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5035,7 +5043,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5058,18 +5066,605 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f>C24/5</f>
+        <v>19.708000000000002</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>98.54</v>
+      </c>
+      <c r="E24" s="2">
+        <f>G24/5</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <f>K24/5</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f t="shared" ref="A25:A55" si="3">C25/5</f>
+        <v>19.708000000000002</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>98.54</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" ref="E25:E39" si="4">G25/5</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" ref="I25:I39" si="5">K25/5</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f t="shared" si="3"/>
+        <v>19.708000000000002</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>98.54</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B30" s="2">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>6</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B31" s="2">
+        <v>7</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>7</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B32" s="2">
+        <v>8</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>8</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B33" s="2">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>9</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B34" s="2">
+        <v>10</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>10</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B35" s="2">
+        <v>11</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>11</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B36" s="2">
+        <v>12</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>12</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B37" s="2">
+        <v>13</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>13</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B38" s="2">
+        <v>14</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>14</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B39" s="2">
+        <v>15</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>15</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B40" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B41" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B42" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B43" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B44" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B45" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B46" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B47" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B48" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B49" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B50" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B51" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B52" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B53" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B54" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="B55" s="2">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="I22:K22"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added some new data to the excel file and ran some tests for the single value or single layer perturbations.
</commit_message>
<xml_diff>
--- a/evaluation data/Accuracy evaluation.xlsx
+++ b/evaluation data/Accuracy evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\github pytorchfi\pytorchfi\evaluation data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4FA2BB-F44B-4CE7-90F0-49C3386C153A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9ED0BD-80EC-4724-80EF-22706B19E8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="1" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiply all values with 1+e" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="63">
   <si>
     <t>Epsilon</t>
   </si>
@@ -216,6 +216,18 @@
   <si>
     <t>densenet121 with CIFAR10 &amp; mul all one layer</t>
   </si>
+  <si>
+    <t>resnet18 with CIFAR10 &amp; mul all one layer</t>
+  </si>
+  <si>
+    <t>resnet18 with CIFAR10 &amp; mul one value each layer</t>
+  </si>
+  <si>
+    <t>value 7</t>
+  </si>
+  <si>
+    <t>layer 2</t>
+  </si>
 </sst>
 </file>
 
@@ -286,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -307,6 +319,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -643,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B82504A-91A0-4B5A-BF2F-634626D37FD7}">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,14 +2127,14 @@
       </c>
       <c r="E50" s="2">
         <f>G50/5</f>
-        <v>69.341999999999999</v>
+        <v>84.61999999999999</v>
       </c>
       <c r="F50" s="2">
         <v>0</v>
       </c>
       <c r="G50">
-        <f>85.95+88.98+86.47+85.31</f>
-        <v>346.71</v>
+        <f>85.95+88.98+86.47+85.31+76.39</f>
+        <v>423.09999999999997</v>
       </c>
       <c r="I50" s="2">
         <f>K50/5</f>
@@ -2145,14 +2158,14 @@
       </c>
       <c r="E51" s="2">
         <f t="shared" ref="E51:E53" si="11">G51/5</f>
-        <v>71.383999999999986</v>
+        <v>86.653999999999996</v>
       </c>
       <c r="F51" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G51">
-        <f>96.16+89.13+86.28+85.35</f>
-        <v>356.91999999999996</v>
+        <f>96.16+89.13+86.28+85.35+76.35</f>
+        <v>433.27</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" ref="I51:I53" si="12">K51/5</f>
@@ -2176,14 +2189,14 @@
       </c>
       <c r="E52" s="2">
         <f t="shared" si="11"/>
-        <v>69.391999999999996</v>
+        <v>84.609999999999985</v>
       </c>
       <c r="F52" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G52">
-        <f>86.23+89.21+86.13+85.39</f>
-        <v>346.96</v>
+        <f>86.23+89.21+86.13+85.39+76.09</f>
+        <v>423.04999999999995</v>
       </c>
       <c r="I52" s="2">
         <f t="shared" si="12"/>
@@ -2207,14 +2220,14 @@
       </c>
       <c r="E53" s="2">
         <f t="shared" si="11"/>
-        <v>69.405999999999992</v>
+        <v>84.559999999999988</v>
       </c>
       <c r="F53" s="6">
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="G53">
-        <f>86.37+89.28+85.99+85.39</f>
-        <v>347.03</v>
+        <f>86.37+89.28+85.99+85.39+75.77</f>
+        <v>422.79999999999995</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" si="12"/>
@@ -2242,14 +2255,14 @@
       </c>
       <c r="E54" s="2">
         <f>G54/5</f>
-        <v>69.443999999999988</v>
+        <v>84.537999999999982</v>
       </c>
       <c r="F54" s="2">
         <v>0.01</v>
       </c>
       <c r="G54">
-        <f>86.51+89.43+85.82+85.46</f>
-        <v>347.21999999999997</v>
+        <f>86.51+89.43+85.82+85.46+75.47</f>
+        <v>422.68999999999994</v>
       </c>
       <c r="I54" s="2">
         <f>K54/5</f>
@@ -2277,14 +2290,14 @@
       </c>
       <c r="E55" s="2">
         <f t="shared" ref="E55:E67" si="14">G55/5</f>
-        <v>69.134</v>
+        <v>83.888000000000005</v>
       </c>
       <c r="F55" s="2">
         <v>0.02</v>
       </c>
       <c r="G55">
-        <f>86.71+89.36+84.42+85.18</f>
-        <v>345.67</v>
+        <f>86.71+89.36+84.42+85.18+73.77</f>
+        <v>419.44</v>
       </c>
       <c r="I55" s="2">
         <f t="shared" ref="I55:I67" si="15">K55/5</f>
@@ -2312,14 +2325,14 @@
       </c>
       <c r="E56" s="2">
         <f t="shared" si="14"/>
-        <v>68.528000000000006</v>
+        <v>82.890000000000015</v>
       </c>
       <c r="F56" s="2">
         <v>0.03</v>
       </c>
       <c r="G56">
-        <f>86.4+89.04+82.78+84.42</f>
-        <v>342.64000000000004</v>
+        <f>86.4+89.04+82.78+84.42+71.81</f>
+        <v>414.45000000000005</v>
       </c>
       <c r="I56" s="2">
         <f t="shared" si="15"/>
@@ -2347,14 +2360,14 @@
       </c>
       <c r="E57" s="2">
         <f t="shared" si="14"/>
-        <v>67.698000000000008</v>
+        <v>81.695999999999998</v>
       </c>
       <c r="F57" s="2">
         <v>0.04</v>
       </c>
       <c r="G57">
-        <f>85.67+88.39+80.68+83.75</f>
-        <v>338.49</v>
+        <f>85.67+88.39+80.68+83.75+69.99</f>
+        <v>408.48</v>
       </c>
       <c r="I57" s="2">
         <f t="shared" si="15"/>
@@ -2382,14 +2395,14 @@
       </c>
       <c r="E58" s="2">
         <f t="shared" si="14"/>
-        <v>66.585999999999999</v>
+        <v>80.152000000000001</v>
       </c>
       <c r="F58" s="2">
         <v>0.05</v>
       </c>
       <c r="G58">
-        <f>84.81+87.44+77.98+82.7</f>
-        <v>332.93</v>
+        <f>84.81+87.44+77.98+82.7+67.83</f>
+        <v>400.76</v>
       </c>
       <c r="I58" s="2">
         <f t="shared" si="15"/>
@@ -2417,14 +2430,14 @@
       </c>
       <c r="E59" s="2">
         <f t="shared" si="14"/>
-        <v>65.225999999999999</v>
+        <v>78.35799999999999</v>
       </c>
       <c r="F59" s="2">
         <v>0.06</v>
       </c>
       <c r="G59">
-        <f>83.33+86.03+75.38+81.39</f>
-        <v>326.13</v>
+        <f>83.33+86.03+75.38+81.39+65.66</f>
+        <v>391.78999999999996</v>
       </c>
       <c r="I59" s="2">
         <f t="shared" si="15"/>
@@ -2452,14 +2465,14 @@
       </c>
       <c r="E60" s="2">
         <f t="shared" si="14"/>
-        <v>63.826000000000001</v>
+        <v>76.465999999999994</v>
       </c>
       <c r="F60" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G60">
-        <f>81.86+84.8+72.54+79.93</f>
-        <v>319.13</v>
+        <f>81.86+84.8+72.54+79.93+63.2</f>
+        <v>382.33</v>
       </c>
       <c r="I60" s="2">
         <f t="shared" si="15"/>
@@ -2487,14 +2500,14 @@
       </c>
       <c r="E61" s="2">
         <f t="shared" si="14"/>
-        <v>62.096000000000004</v>
+        <v>74.234000000000009</v>
       </c>
       <c r="F61" s="2">
         <v>0.08</v>
       </c>
       <c r="G61">
-        <f>79.73+83.29+69.18+78.28</f>
-        <v>310.48</v>
+        <f>79.73+83.29+69.18+78.28+60.69</f>
+        <v>371.17</v>
       </c>
       <c r="I61" s="2">
         <f t="shared" si="15"/>
@@ -2522,14 +2535,14 @@
       </c>
       <c r="E62" s="2">
         <f t="shared" si="14"/>
-        <v>60.327999999999996</v>
+        <v>71.994</v>
       </c>
       <c r="F62" s="2">
         <v>0.09</v>
       </c>
       <c r="G62">
-        <f>77.83+81.74+65.7+76.37</f>
-        <v>301.64</v>
+        <f>77.83+81.74+65.7+76.37+58.33</f>
+        <v>359.96999999999997</v>
       </c>
       <c r="I62" s="2">
         <f t="shared" si="15"/>
@@ -2557,14 +2570,14 @@
       </c>
       <c r="E63" s="2">
         <f t="shared" si="14"/>
-        <v>58.632000000000005</v>
+        <v>69.830000000000013</v>
       </c>
       <c r="F63" s="2">
         <v>0.1</v>
       </c>
       <c r="G63">
-        <f>76.02+80.22+62.41+74.51</f>
-        <v>293.16000000000003</v>
+        <f>76.02+80.22+62.41+74.51+55.99</f>
+        <v>349.15000000000003</v>
       </c>
       <c r="I63" s="2">
         <f t="shared" si="15"/>
@@ -2592,14 +2605,14 @@
       </c>
       <c r="E64" s="2">
         <f t="shared" si="14"/>
-        <v>39.673999999999999</v>
+        <v>46.958000000000006</v>
       </c>
       <c r="F64" s="2">
         <v>0.2</v>
       </c>
       <c r="G64">
-        <f>53.35+60.42+35.23+49.37</f>
-        <v>198.37</v>
+        <f>53.35+60.42+35.23+49.37+36.42</f>
+        <v>234.79000000000002</v>
       </c>
       <c r="I64" s="2">
         <f t="shared" si="15"/>
@@ -2627,14 +2640,14 @@
       </c>
       <c r="E65" s="2">
         <f t="shared" si="14"/>
-        <v>22.582000000000001</v>
+        <v>27.121999999999996</v>
       </c>
       <c r="F65" s="2">
         <v>0.3</v>
       </c>
       <c r="G65">
-        <f>30.14+31.8+23.66+27.31</f>
-        <v>112.91</v>
+        <f>30.14+31.8+23.66+27.31+22.7</f>
+        <v>135.60999999999999</v>
       </c>
       <c r="I65" s="2">
         <f t="shared" si="15"/>
@@ -2662,14 +2675,14 @@
       </c>
       <c r="E66" s="2">
         <f t="shared" si="14"/>
-        <v>15.457999999999998</v>
+        <v>19.167999999999999</v>
       </c>
       <c r="F66" s="2">
         <v>0.4</v>
       </c>
       <c r="G66">
-        <f>20.97+18.74+17.93+19.65</f>
-        <v>77.289999999999992</v>
+        <f>20.97+18.74+17.93+19.65+18.55</f>
+        <v>95.839999999999989</v>
       </c>
       <c r="I66" s="2">
         <f t="shared" si="15"/>
@@ -2697,14 +2710,14 @@
       </c>
       <c r="E67" s="2">
         <f t="shared" si="14"/>
-        <v>11.416</v>
+        <v>14.441999999999998</v>
       </c>
       <c r="F67" s="2">
         <v>0.5</v>
       </c>
       <c r="G67">
-        <f>15.53+11.86+11.36+18.33</f>
-        <v>57.08</v>
+        <f>15.53+11.86+11.36+18.33+15.13</f>
+        <v>72.209999999999994</v>
       </c>
       <c r="I67" s="2">
         <f t="shared" si="15"/>
@@ -5108,7 +5121,7 @@
       </c>
       <c r="G157" s="2">
         <f>E50</f>
-        <v>69.341999999999999</v>
+        <v>84.61999999999999</v>
       </c>
       <c r="I157" t="s">
         <v>41</v>
@@ -5252,18 +5265,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF5FB46-611D-4C69-BF4D-AAF86A3749DC}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -5278,10 +5292,10 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -5296,9 +5310,7 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
@@ -5327,15 +5339,9 @@
       <c r="H3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -5360,13 +5366,8 @@
         <f>63.73+63+86.78+76.95+82.18</f>
         <v>372.64</v>
       </c>
-      <c r="I4" s="2">
-        <f>K4/5</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -5391,13 +5392,8 @@
         <f>89.97</f>
         <v>89.97</v>
       </c>
-      <c r="I5" s="2">
-        <f>K5/5</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.01</v>
-      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -5422,13 +5418,8 @@
         <f>89.96</f>
         <v>89.96</v>
       </c>
-      <c r="I6" s="2">
-        <f t="shared" ref="I6:I18" si="3">K6/5</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.02</v>
-      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -5453,13 +5444,8 @@
         <f>89.96</f>
         <v>89.96</v>
       </c>
-      <c r="I7" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.03</v>
-      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -5484,13 +5470,8 @@
         <f>89.93</f>
         <v>89.93</v>
       </c>
-      <c r="I8" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.04</v>
-      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -5515,13 +5496,8 @@
         <f>89.92</f>
         <v>89.92</v>
       </c>
-      <c r="I9" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.05</v>
-      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -5546,13 +5522,8 @@
         <f>89.88</f>
         <v>89.88</v>
       </c>
-      <c r="I10" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.06</v>
-      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -5577,13 +5548,8 @@
         <f>89.85</f>
         <v>89.85</v>
       </c>
-      <c r="I11" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -5608,13 +5574,8 @@
         <f>89.81</f>
         <v>89.81</v>
       </c>
-      <c r="I12" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.08</v>
-      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -5639,13 +5600,8 @@
         <f>89.77</f>
         <v>89.77</v>
       </c>
-      <c r="I13" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.09</v>
-      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -5670,13 +5626,8 @@
         <f>89.73</f>
         <v>89.73</v>
       </c>
-      <c r="I14" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -5701,13 +5652,8 @@
         <f>89.45</f>
         <v>89.45</v>
       </c>
-      <c r="I15" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.2</v>
-      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -5718,7 +5664,7 @@
         <v>0.3</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:C17" si="4">90.98</f>
+        <f t="shared" ref="C16:C17" si="3">90.98</f>
         <v>90.98</v>
       </c>
       <c r="E16" s="2">
@@ -5732,13 +5678,8 @@
         <f>89.45</f>
         <v>89.45</v>
       </c>
-      <c r="I16" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -5749,7 +5690,7 @@
         <v>0.4</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>90.98</v>
       </c>
       <c r="E17" s="2">
@@ -5763,13 +5704,8 @@
         <f>89.1</f>
         <v>89.1</v>
       </c>
-      <c r="I17" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.4</v>
-      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
@@ -5794,20 +5730,428 @@
         <f>G17</f>
         <v>89.1</v>
       </c>
-      <c r="I18" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="2">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <f>C23/5</f>
+        <v>17.350000000000001</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>86.75</f>
+        <v>86.75</v>
+      </c>
+      <c r="E23" s="2">
+        <f>G23/5</f>
+        <v>18.369999999999997</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>91.85</f>
+        <v>91.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f>C24/5</f>
+        <v>17.350000000000001</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="C24">
+        <f>86.75</f>
+        <v>86.75</v>
+      </c>
+      <c r="E24" s="2">
+        <f>G24/5</f>
+        <v>18.368000000000002</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G24">
+        <f>91.84</f>
+        <v>91.84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f t="shared" ref="A25:A37" si="4">C25/5</f>
+        <v>17.350000000000001</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="C25">
+        <f>86.75</f>
+        <v>86.75</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" ref="E25:E37" si="5">G25/5</f>
+        <v>19.765999999999998</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="G25">
+        <f>98.83</f>
+        <v>98.83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="C26">
+        <f>86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="5"/>
+        <v>19.765999999999998</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G27" si="6">98.83</f>
+        <v>98.83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C28" si="7">86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="5"/>
+        <v>19.765999999999998</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="6"/>
+        <v>98.83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="7"/>
+        <v>86.76</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="5"/>
+        <v>18.363999999999997</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G28">
+        <f>91.82</f>
+        <v>91.82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="C29">
+        <f>86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="5"/>
+        <v>18.363999999999997</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="G29">
+        <f>91.82</f>
+        <v>91.82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B30" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C30">
+        <f>86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="5"/>
+        <v>18.362000000000002</v>
+      </c>
+      <c r="F30" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G30">
+        <f>91.81</f>
+        <v>91.81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="C31">
+        <f>86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="5"/>
+        <v>18.362000000000002</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:G32" si="8">91.81</f>
+        <v>91.81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="C32">
+        <f>86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="5"/>
+        <v>18.362000000000002</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="8"/>
+        <v>91.81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <f t="shared" si="4"/>
+        <v>17.352</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C33">
+        <f>86.76</f>
+        <v>86.76</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="5"/>
+        <v>18.36</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="G33">
+        <f>91.8</f>
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <f t="shared" si="4"/>
+        <v>17.350000000000001</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C34">
+        <f>86.75</f>
+        <v>86.75</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="5"/>
+        <v>18.344000000000001</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G34">
+        <f>91.72</f>
+        <v>91.72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <f t="shared" si="4"/>
+        <v>17.347999999999999</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="C35">
+        <f>86.74</f>
+        <v>86.74</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="5"/>
+        <v>18.308</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="G35">
+        <f>91.54</f>
+        <v>91.54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <f t="shared" si="4"/>
+        <v>17.346</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C36">
+        <f>86.73</f>
+        <v>86.73</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="5"/>
+        <v>18.231999999999999</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G36">
+        <f>91.16</f>
+        <v>91.16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <f t="shared" si="4"/>
+        <v>17.347999999999999</v>
+      </c>
+      <c r="B37" s="2">
         <v>0.5</v>
       </c>
+      <c r="C37">
+        <f>86.74</f>
+        <v>86.74</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="5"/>
+        <v>18.204000000000001</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G37">
+        <f>91.02</f>
+        <v>91.02</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:K1"/>
+  <mergeCells count="7">
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="E21:G21"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="I2:K2"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5817,8 +6161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A2FD27-2957-4E5E-9083-A23CA00D16E3}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Created functions for evaluating different perturbation methods and changed some graphs
</commit_message>
<xml_diff>
--- a/evaluation data/Accuracy evaluation.xlsx
+++ b/evaluation data/Accuracy evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\github pytorchfi\evaluation data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Bachelorarbeit\github pytorchfi\pytorchfi\evaluation data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3522CF0-8A32-45ED-B973-C93E5E7EF555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4898C6-50D5-41FA-A593-D5BEA1C0937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="885" windowWidth="15555" windowHeight="14715" firstSheet="3" activeTab="4" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
+    <workbookView xWindow="32040" yWindow="1365" windowWidth="15555" windowHeight="14715" xr2:uid="{F7DC7ED8-E023-4EB5-A7C2-BCA1138A1D29}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiply neuron values by 1+e" sheetId="1" r:id="rId1"/>
@@ -4884,10 +4884,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="106"/>
+      <c14:style val="104"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="6"/>
+      <c:style val="4"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -4912,7 +4912,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>DenseNet121 with CIFAR100 &amp; bit flip in layer 4</a:t>
+              <a:t>GoogLeNet with CIFAR10 &amp; bit flip in layer 0</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4959,7 +4959,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4970,11 +4970,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -5029,75 +5029,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Single weight bitlflip'!$E$20:$E$32</c:f>
+              <c:f>'Single weight bitlflip'!$A$20:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>78.209999999999994</c:v>
+                  <c:v>86.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.66</c:v>
+                  <c:v>84.22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>77.62</c:v>
+                  <c:v>83.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.510000000000005</c:v>
+                  <c:v>72.56</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.099999999999994</c:v>
+                  <c:v>70.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>74.790000000000006</c:v>
+                  <c:v>44.45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.869999999999997</c:v>
+                  <c:v>30.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.39</c:v>
+                  <c:v>12.17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.17</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.32</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.34</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.34</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:filteredSeriesTitle>
-                <c15:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'Single neuron bitflip'!#REF!</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>#REF!</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c15:tx>
-              </c15:filteredSeriesTitle>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3037-4563-8CA1-4F9D384F1C4A}"/>
             </c:ext>
@@ -6072,7 +6051,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>84.61999999999999</c:v>
+                  <c:v>86.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>86.653999999999996</c:v>
@@ -7398,7 +7377,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-AT"/>
-              <a:t>Evaluation of original models with CIFAR100</a:t>
+              <a:t>Evaluation of original models with CIFAR10</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7444,7 +7423,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5">
+              <a:schemeClr val="accent2">
                 <a:lumMod val="40000"/>
                 <a:lumOff val="60000"/>
               </a:schemeClr>
@@ -7538,24 +7517,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Multiply neuron values by 1+e'!$K$155:$K$159</c:f>
+              <c:f>'Multiply neuron values by 1+e'!$G$155:$G$159</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>66.687999999999988</c:v>
+                  <c:v>83.304000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.207999999999998</c:v>
+                  <c:v>90.347999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.179999999999993</c:v>
+                  <c:v>86.82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.03</c:v>
+                  <c:v>90.92</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79.777999999999992</c:v>
+                  <c:v>87.483999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7691,7 +7670,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
-          <c:min val="60"/>
+          <c:min val="70"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -7986,7 +7965,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>84.61999999999999</c:v>
+                  <c:v>86.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>86.653999999999996</c:v>
@@ -9885,8 +9864,8 @@
 </file>
 
 <file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
-  <a:schemeClr val="accent4"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
+  <a:schemeClr val="accent2"/>
 </cs:colorStyle>
 </file>
 
@@ -20809,8 +20788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B82504A-91A0-4B5A-BF2F-634626D37FD7}">
   <dimension ref="A1:K161"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L178" sqref="L178"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22278,14 +22257,14 @@
       </c>
       <c r="E50" s="2">
         <f>G50/5</f>
-        <v>84.61999999999999</v>
+        <v>86.82</v>
       </c>
       <c r="F50" s="2">
         <v>0</v>
       </c>
       <c r="G50">
-        <f>85.95+88.98+86.47+85.31+76.39</f>
-        <v>423.09999999999997</v>
+        <f>96.95+88.98+86.47+85.31+76.39</f>
+        <v>434.09999999999997</v>
       </c>
       <c r="I50" s="2">
         <f>K50/5</f>
@@ -25192,7 +25171,7 @@
       </c>
       <c r="G157" s="2">
         <f>E50</f>
-        <v>84.61999999999999</v>
+        <v>86.82</v>
       </c>
       <c r="I157" t="s">
         <v>83</v>
@@ -26355,7 +26334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F79264-4CD7-4986-94A3-1DEF854F93EC}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
@@ -27541,8 +27520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A2FD27-2957-4E5E-9083-A23CA00D16E3}">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView topLeftCell="G27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView topLeftCell="E27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28131,7 +28110,8 @@
         <v>46</v>
       </c>
       <c r="E22" s="2">
-        <v>81.34</v>
+        <f>86.82</f>
+        <v>86.82</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>46</v>
@@ -29563,8 +29543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA7F4C0-5905-4A01-A765-CDF8CD5C9776}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29862,8 +29842,8 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f>84.62</f>
-        <v>84.62</v>
+        <f>86.82</f>
+        <v>86.82</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>46</v>

</xml_diff>